<commit_message>
Modified gummy data key
</commit_message>
<xml_diff>
--- a/input/data_keys/gummy_data_key.xlsx
+++ b/input/data_keys/gummy_data_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gsk-centrum-classic\input\data_keys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201B6470-1D62-4D89-9FE7-74315A3A6942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C6A0A2-134F-45F7-858C-B161217769FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Info" sheetId="1" r:id="rId1"/>
@@ -590,10 +590,10 @@
     <t>A_First Bite Hardness</t>
   </si>
   <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
+    <t>Min_val</t>
+  </si>
+  <si>
+    <t>Max_val</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -699,7 +699,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,7 +982,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B10"/>
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,20 +1160,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B910EDBC-ABD3-430B-886D-9E756DEF056D}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.140625" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" customWidth="1"/>
+    <col min="4" max="5" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>35.700000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>34.65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>40.950000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1273,10 +1267,10 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>10.591666666666701</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>52.575000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>81.900000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>17.850000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>70.349999999999994</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>62.475000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,10 +1352,10 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>5.125</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>57.375</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,10 +1369,10 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>3.5416666666666701</v>
       </c>
       <c r="E12">
-        <v>100</v>
+        <v>46.625</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,10 +1403,10 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="E14">
-        <v>100</v>
+        <v>55.633333333333297</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1426,10 +1420,10 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>11.3333333333333</v>
       </c>
       <c r="E15">
-        <v>100</v>
+        <v>55.3333333333333</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>100</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>43.05</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1477,10 +1471,10 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>7.6333333333333302</v>
       </c>
       <c r="E18">
-        <v>100</v>
+        <v>37.700000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1494,10 +1488,10 @@
         <v>5</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>2.18333333333333</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>64.150000000000006</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>100</v>
+        <v>21.35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>100</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>100</v>
+        <v>13.8588141025641</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>100</v>
+        <v>31.7871794871795</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>17.014743589743599</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1646,11 +1640,11 @@
       <c r="C28">
         <v>7</v>
       </c>
-      <c r="D28" s="7">
-        <v>-9.9999999999999997E+98</v>
-      </c>
-      <c r="E28" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="D28">
+        <v>-460.27955181715299</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1663,11 +1657,11 @@
       <c r="C29">
         <v>7</v>
       </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="D29">
+        <v>38.253010022841302</v>
+      </c>
+      <c r="E29">
+        <v>21176.385364753201</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1680,11 +1674,11 @@
       <c r="C30">
         <v>7</v>
       </c>
-      <c r="D30" s="7">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="D30">
+        <v>0.45384820957368799</v>
+      </c>
+      <c r="E30">
+        <v>0.87879933661402998</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1697,11 +1691,11 @@
       <c r="C31">
         <v>7</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="E31">
+        <v>25513.339510966802</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1714,11 +1708,11 @@
       <c r="C32">
         <v>7</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32">
         <v>0</v>
       </c>
-      <c r="E32" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="E32">
+        <v>35978.039452392499</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1731,11 +1725,11 @@
       <c r="C33">
         <v>7</v>
       </c>
-      <c r="D33" s="7">
-        <v>-9.9999999999999997E+98</v>
-      </c>
-      <c r="E33" s="7">
-        <v>0</v>
+      <c r="D33">
+        <v>-638.81177887917397</v>
+      </c>
+      <c r="E33">
+        <v>-276.62056806683199</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1748,11 +1742,11 @@
       <c r="C34">
         <v>7</v>
       </c>
-      <c r="D34" s="7">
-        <v>-9.9999999999999997E+98</v>
-      </c>
-      <c r="E34" s="7">
-        <v>0</v>
+      <c r="D34">
+        <v>-379.56949223212803</v>
+      </c>
+      <c r="E34">
+        <v>-190.16778661728199</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,11 +1759,11 @@
       <c r="C35">
         <v>7</v>
       </c>
-      <c r="D35" s="7">
-        <v>0</v>
-      </c>
-      <c r="E35" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="D35">
+        <v>18.407415045495</v>
+      </c>
+      <c r="E35">
+        <v>57.223971025907097</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1782,11 +1776,11 @@
       <c r="C36">
         <v>7</v>
       </c>
-      <c r="D36" s="7">
-        <v>0</v>
-      </c>
-      <c r="E36" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="D36">
+        <v>67.092896928727399</v>
+      </c>
+      <c r="E36">
+        <v>98.062014109751104</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1799,11 +1793,11 @@
       <c r="C37">
         <v>7</v>
       </c>
-      <c r="D37" s="7">
-        <v>0</v>
-      </c>
-      <c r="E37" s="7">
-        <v>9.9999999999999997E+98</v>
+      <c r="D37">
+        <v>216.366249903115</v>
+      </c>
+      <c r="E37">
+        <v>31267.260024751999</v>
       </c>
     </row>
   </sheetData>
@@ -1879,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7018D01-5AC2-40A3-921B-EAF020F08594}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:XFD74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3056,7 +3050,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>